<commit_message>
Updated ISL model - 2025-08-01 00:25
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/source_data/VerveStacks_ISL.xlsx
+++ b/VerveStacks_ISL/source_data/VerveStacks_ISL.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32A84AE-6EA3-44D9-A5C7-BD9941E27460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590175CE-CA5D-4F8B-BDA8-DD531172B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="iamc_data" sheetId="16" r:id="rId1"/>
-    <sheet name="iamc_charts" sheetId="15" r:id="rId2"/>
-    <sheet name="weo_pg" sheetId="14" r:id="rId3"/>
-    <sheet name="re_targets" sheetId="13" r:id="rId4"/>
-    <sheet name="ccs_retrofits" sheetId="12" r:id="rId5"/>
-    <sheet name="Calibration" sheetId="11" r:id="rId6"/>
-    <sheet name="existing_stock" sheetId="10" r:id="rId7"/>
+    <sheet name="iamc_data" sheetId="23" r:id="rId1"/>
+    <sheet name="iamc_charts" sheetId="22" r:id="rId2"/>
+    <sheet name="weo_pg" sheetId="21" r:id="rId3"/>
+    <sheet name="re_targets" sheetId="20" r:id="rId4"/>
+    <sheet name="ccs_retrofits" sheetId="19" r:id="rId5"/>
+    <sheet name="Calibration" sheetId="18" r:id="rId6"/>
+    <sheet name="existing_stock" sheetId="17" r:id="rId7"/>
     <sheet name="historical_data" sheetId="4" r:id="rId8"/>
     <sheet name="system_settings" sheetId="1" r:id="rId9"/>
   </sheets>
@@ -890,7 +890,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E9B230D-CFA8-A491-D600-F9051A306A6A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8941112E-70E7-1FC1-96DB-A94D915BFBE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1241,7 +1241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEEB8B5-53B2-4271-8FD2-54CCA59A77C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3CEA65-DDE2-4CDC-AD34-08A233FB3864}">
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3604,7 +3604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1134144-BED7-4C6E-8203-FCDFBAD4D4A7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAD6154-BA19-4E5E-933D-6CDBBD901B21}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3617,7 +3617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2568F822-72F8-4968-ACB9-3C4CBD386E2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9346D617-A190-4305-BF4F-98CDA7F99FBF}">
   <dimension ref="A1:H209"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8752,7 +8752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B21D15-BF3C-494D-8693-09D6F0763570}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE806BD-037E-47C4-908B-16A100760E00}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8835,7 +8835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1CA371-AACC-4B35-8933-D3E5B26CA6DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093C6D5-A287-4FBD-A9E7-B262E7043734}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8877,7 +8877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD0EAED-64C5-4760-BE69-ACC85B44E559}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF992A65-69A7-4E20-9888-C89B3FAC1E64}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9223,7 +9223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BEDDEB-27F9-4A25-AAEE-2B5414414533}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3220A85-DA37-49E1-80DB-11D2E3A68BF1}">
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 00:26
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/source_data/VerveStacks_ISL.xlsx
+++ b/VerveStacks_ISL/source_data/VerveStacks_ISL.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590175CE-CA5D-4F8B-BDA8-DD531172B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E66D09D-F899-47A8-B9FC-EE2AE3724E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="iamc_data" sheetId="23" r:id="rId1"/>
-    <sheet name="iamc_charts" sheetId="22" r:id="rId2"/>
-    <sheet name="weo_pg" sheetId="21" r:id="rId3"/>
-    <sheet name="re_targets" sheetId="20" r:id="rId4"/>
-    <sheet name="ccs_retrofits" sheetId="19" r:id="rId5"/>
-    <sheet name="Calibration" sheetId="18" r:id="rId6"/>
-    <sheet name="existing_stock" sheetId="17" r:id="rId7"/>
+    <sheet name="iamc_data" sheetId="30" r:id="rId1"/>
+    <sheet name="iamc_charts" sheetId="29" r:id="rId2"/>
+    <sheet name="weo_pg" sheetId="28" r:id="rId3"/>
+    <sheet name="re_targets" sheetId="27" r:id="rId4"/>
+    <sheet name="ccs_retrofits" sheetId="26" r:id="rId5"/>
+    <sheet name="Calibration" sheetId="25" r:id="rId6"/>
+    <sheet name="existing_stock" sheetId="24" r:id="rId7"/>
     <sheet name="historical_data" sheetId="4" r:id="rId8"/>
     <sheet name="system_settings" sheetId="1" r:id="rId9"/>
   </sheets>
@@ -890,7 +890,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8941112E-70E7-1FC1-96DB-A94D915BFBE0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54682B87-1893-F4AA-81C3-BD90CE01187A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1241,7 +1241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3CEA65-DDE2-4CDC-AD34-08A233FB3864}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C842500-3978-404A-9B27-0769257BC425}">
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3604,7 +3604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAD6154-BA19-4E5E-933D-6CDBBD901B21}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69079D8E-25B5-4EE9-BA8B-8007FC2DA9BC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3617,7 +3617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9346D617-A190-4305-BF4F-98CDA7F99FBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C46FE1C-EC0A-4294-A6AE-1B627567E0CC}">
   <dimension ref="A1:H209"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8752,7 +8752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE806BD-037E-47C4-908B-16A100760E00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491B6EB-92FE-4DD3-9ED8-F4119779D493}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8835,7 +8835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E093C6D5-A287-4FBD-A9E7-B262E7043734}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAADC93-23CF-4A09-8149-EDAADFF6D639}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8877,7 +8877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF992A65-69A7-4E20-9888-C89B3FAC1E64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C229F0B9-C58A-4751-AC87-238AB7126705}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9223,7 +9223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3220A85-DA37-49E1-80DB-11D2E3A68BF1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F840402-4293-4F09-B712-21A02D38C24A}">
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ISL model - 2025-08-01 00:27
</commit_message>
<xml_diff>
--- a/VerveStacks_ISL/source_data/VerveStacks_ISL.xlsx
+++ b/VerveStacks_ISL/source_data/VerveStacks_ISL.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E66D09D-F899-47A8-B9FC-EE2AE3724E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4760B1B-DE7F-47CA-BC35-44D7B7869F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="iamc_data" sheetId="30" r:id="rId1"/>
-    <sheet name="iamc_charts" sheetId="29" r:id="rId2"/>
-    <sheet name="weo_pg" sheetId="28" r:id="rId3"/>
-    <sheet name="re_targets" sheetId="27" r:id="rId4"/>
-    <sheet name="ccs_retrofits" sheetId="26" r:id="rId5"/>
-    <sheet name="Calibration" sheetId="25" r:id="rId6"/>
-    <sheet name="existing_stock" sheetId="24" r:id="rId7"/>
+    <sheet name="iamc_data" sheetId="37" r:id="rId1"/>
+    <sheet name="iamc_charts" sheetId="36" r:id="rId2"/>
+    <sheet name="weo_pg" sheetId="35" r:id="rId3"/>
+    <sheet name="re_targets" sheetId="34" r:id="rId4"/>
+    <sheet name="ccs_retrofits" sheetId="33" r:id="rId5"/>
+    <sheet name="Calibration" sheetId="32" r:id="rId6"/>
+    <sheet name="existing_stock" sheetId="31" r:id="rId7"/>
     <sheet name="historical_data" sheetId="4" r:id="rId8"/>
     <sheet name="system_settings" sheetId="1" r:id="rId9"/>
   </sheets>
@@ -890,7 +890,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54682B87-1893-F4AA-81C3-BD90CE01187A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52F90960-480C-88B7-AC57-54AB71A38F13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1241,7 +1241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C842500-3978-404A-9B27-0769257BC425}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF7E3AD8-1751-4AFC-BC00-74B1117227B5}">
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -3604,7 +3604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69079D8E-25B5-4EE9-BA8B-8007FC2DA9BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB9150F-31CE-4A45-B137-1CBCDF5096C5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3617,7 +3617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C46FE1C-EC0A-4294-A6AE-1B627567E0CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBECEA1-E0EB-4CEE-A206-75AB5229E884}">
   <dimension ref="A1:H209"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8752,7 +8752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7491B6EB-92FE-4DD3-9ED8-F4119779D493}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608BFBE7-1B18-4D26-A792-A606A975D563}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8835,7 +8835,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAADC93-23CF-4A09-8149-EDAADFF6D639}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1C5797-5D66-4CBC-9FE3-DD1EADADCBA7}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8877,7 +8877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C229F0B9-C58A-4751-AC87-238AB7126705}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83953002-9F5E-49BE-82B0-3B18300F22A2}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9223,7 +9223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F840402-4293-4F09-B712-21A02D38C24A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98A27B1-307E-4496-B8FE-9E223FFBEA34}">
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>